<commit_message>
Final updates RP3 DB
</commit_message>
<xml_diff>
--- a/static/download/2020/RP3_FLT_EFF_2020_Jan_Apr.xlsx
+++ b/static/download/2020/RP3_FLT_EFF_2020_Jan_Apr.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="153">
   <si>
     <t>Data source</t>
   </si>
@@ -347,7 +347,7 @@
     <t>Dif.</t>
   </si>
   <si>
-    <t>SES Area (RP2)</t>
+    <t>SES Area</t>
   </si>
   <si>
     <t>Baltic FAB</t>
@@ -843,14 +843,6 @@
       <bottom/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -870,6 +862,14 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left/>
@@ -891,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -970,13 +970,13 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -1054,45 +1054,39 @@
     <xf borderId="18" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="18" fillId="3" fontId="23" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="19" fillId="3" fontId="22" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="20" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="3" fontId="22" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="20" fillId="3" fontId="23" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="21" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="18" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="21" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="20" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="22" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="21" fillId="3" fontId="23" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="16" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="19" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="21" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -1129,7 +1123,7 @@
     <xf borderId="7" fillId="4" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="7" fillId="6" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="6" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1141,7 +1135,10 @@
     <xf borderId="7" fillId="6" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="21" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="20" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="3" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1386,13 +1383,13 @@
       <c r="D6" s="26">
         <v>0.0486</v>
       </c>
-      <c r="E6" s="27">
-        <v>0.0</v>
+      <c r="E6" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="F6" s="26">
         <v>0.0284</v>
       </c>
-      <c r="G6" s="28"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="23" t="s">
@@ -1407,11 +1404,11 @@
       <c r="D7" s="26">
         <v>0.0485</v>
       </c>
-      <c r="E7" s="27"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="26">
         <v>0.0293</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="23" t="s">
@@ -1426,17 +1423,17 @@
       <c r="D8" s="26">
         <v>0.0472</v>
       </c>
-      <c r="E8" s="27"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="26">
         <v>0.0279</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="25">
@@ -1445,11 +1442,11 @@
       <c r="D9" s="26">
         <v>0.0469</v>
       </c>
-      <c r="E9" s="27"/>
+      <c r="E9" s="26"/>
       <c r="F9" s="26">
         <v>0.0286</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="23" t="s">
@@ -1464,11 +1461,13 @@
       <c r="D10" s="26">
         <v>0.0466</v>
       </c>
-      <c r="E10" s="27"/>
+      <c r="E10" s="29">
+        <v>0.043</v>
+      </c>
       <c r="F10" s="26">
         <v>0.0294</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="27">
         <v>0.0253</v>
       </c>
     </row>
@@ -1481,9 +1480,9 @@
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="26"/>
-      <c r="G11" s="28">
+      <c r="G11" s="27">
         <v>0.0247</v>
       </c>
     </row>
@@ -1496,9 +1495,9 @@
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="26"/>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <v>0.024</v>
       </c>
     </row>
@@ -1511,9 +1510,9 @@
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="26"/>
-      <c r="G13" s="28">
+      <c r="G13" s="27">
         <v>0.024</v>
       </c>
     </row>
@@ -1526,9 +1525,9 @@
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="26"/>
-      <c r="G14" s="28">
+      <c r="G14" s="27">
         <v>0.024</v>
       </c>
     </row>
@@ -1662,7 +1661,7 @@
       <c r="B7" s="55">
         <v>0.0471</v>
       </c>
-      <c r="C7" s="56"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="55">
         <v>0.0285</v>
       </c>
@@ -1677,7 +1676,7 @@
       <c r="B8" s="55">
         <v>0.047</v>
       </c>
-      <c r="C8" s="56"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="55">
         <v>0.0286</v>
       </c>
@@ -1692,7 +1691,7 @@
       <c r="B9" s="55">
         <v>0.0469</v>
       </c>
-      <c r="C9" s="56"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="55">
         <v>0.0286</v>
       </c>
@@ -1707,7 +1706,7 @@
       <c r="B10" s="55">
         <v>0.0469</v>
       </c>
-      <c r="C10" s="56"/>
+      <c r="C10" s="55"/>
       <c r="D10" s="55">
         <v>0.0286</v>
       </c>
@@ -1722,8 +1721,8 @@
       <c r="B11" s="55">
         <v>0.0468</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="57">
+      <c r="C11" s="55"/>
+      <c r="D11" s="56">
         <v>0.0287</v>
       </c>
       <c r="E11" s="53">
@@ -1737,8 +1736,8 @@
       <c r="B12" s="55">
         <v>0.0468</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57">
+      <c r="C12" s="55"/>
+      <c r="D12" s="56">
         <v>0.0289</v>
       </c>
       <c r="E12" s="53">
@@ -1752,8 +1751,8 @@
       <c r="B13" s="55">
         <v>0.0468</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57">
+      <c r="C13" s="55"/>
+      <c r="D13" s="56">
         <v>0.029</v>
       </c>
       <c r="E13" s="53">
@@ -1767,8 +1766,8 @@
       <c r="B14" s="55">
         <v>0.0468</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57">
+      <c r="C14" s="55"/>
+      <c r="D14" s="56">
         <v>0.0292</v>
       </c>
       <c r="E14" s="53">
@@ -1782,8 +1781,8 @@
       <c r="B15" s="55">
         <v>0.0468</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57">
+      <c r="C15" s="55"/>
+      <c r="D15" s="56">
         <v>0.0293</v>
       </c>
       <c r="E15" s="53">
@@ -1794,11 +1793,11 @@
       <c r="A16" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="58">
+      <c r="B16" s="57">
         <v>0.0467</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="57">
+      <c r="C16" s="55"/>
+      <c r="D16" s="56">
         <v>0.0293</v>
       </c>
       <c r="E16" s="53">
@@ -1806,14 +1805,14 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="61">
+      <c r="B17" s="59">
         <v>0.0468</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63">
+      <c r="C17" s="55"/>
+      <c r="D17" s="60">
         <v>0.0295</v>
       </c>
       <c r="E17" s="53">
@@ -1827,7 +1826,9 @@
       <c r="B18" s="51">
         <v>0.0468</v>
       </c>
-      <c r="C18" s="64"/>
+      <c r="C18" s="51">
+        <v>0.0432</v>
+      </c>
       <c r="D18" s="51">
         <v>0.0295</v>
       </c>
@@ -1842,7 +1843,9 @@
       <c r="B19" s="55">
         <v>0.0468</v>
       </c>
-      <c r="C19" s="56"/>
+      <c r="C19" s="55">
+        <v>0.0432</v>
+      </c>
       <c r="D19" s="55">
         <v>0.0295</v>
       </c>
@@ -1857,7 +1860,9 @@
       <c r="B20" s="55">
         <v>0.0467</v>
       </c>
-      <c r="C20" s="56"/>
+      <c r="C20" s="55">
+        <v>0.0431</v>
+      </c>
       <c r="D20" s="55">
         <v>0.0294</v>
       </c>
@@ -1872,7 +1877,9 @@
       <c r="B21" s="55">
         <v>0.0466</v>
       </c>
-      <c r="C21" s="56"/>
+      <c r="C21" s="55">
+        <v>0.043</v>
+      </c>
       <c r="D21" s="55">
         <v>0.0294</v>
       </c>
@@ -1885,7 +1892,7 @@
         <v>45</v>
       </c>
       <c r="B22" s="55"/>
-      <c r="C22" s="56"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="55"/>
       <c r="E22" s="53"/>
     </row>
@@ -1894,8 +1901,8 @@
         <v>46</v>
       </c>
       <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="57"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="56"/>
       <c r="E23" s="53"/>
     </row>
     <row r="24">
@@ -1903,8 +1910,8 @@
         <v>47</v>
       </c>
       <c r="B24" s="55"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="57"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="56"/>
       <c r="E24" s="53"/>
     </row>
     <row r="25">
@@ -1912,8 +1919,8 @@
         <v>48</v>
       </c>
       <c r="B25" s="55"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="57"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="56"/>
       <c r="E25" s="53"/>
     </row>
     <row r="26">
@@ -1921,8 +1928,8 @@
         <v>49</v>
       </c>
       <c r="B26" s="55"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="57"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="53"/>
     </row>
     <row r="27">
@@ -1930,26 +1937,26 @@
         <v>50</v>
       </c>
       <c r="B27" s="55"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="57"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="56"/>
       <c r="E27" s="53"/>
     </row>
     <row r="28">
       <c r="A28" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="57"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="56"/>
       <c r="E28" s="53"/>
     </row>
     <row r="29">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="63"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="53"/>
     </row>
     <row r="30">
@@ -1957,7 +1964,7 @@
         <v>53</v>
       </c>
       <c r="B30" s="51"/>
-      <c r="C30" s="64"/>
+      <c r="C30" s="66"/>
       <c r="D30" s="51"/>
       <c r="E30" s="53"/>
     </row>
@@ -1966,7 +1973,7 @@
         <v>54</v>
       </c>
       <c r="B31" s="55"/>
-      <c r="C31" s="56"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="55"/>
       <c r="E31" s="53"/>
     </row>
@@ -1975,7 +1982,7 @@
         <v>55</v>
       </c>
       <c r="B32" s="55"/>
-      <c r="C32" s="56"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="55"/>
       <c r="E32" s="53"/>
     </row>
@@ -1984,7 +1991,7 @@
         <v>56</v>
       </c>
       <c r="B33" s="55"/>
-      <c r="C33" s="56"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="55"/>
       <c r="E33" s="53"/>
     </row>
@@ -1993,7 +2000,7 @@
         <v>57</v>
       </c>
       <c r="B34" s="55"/>
-      <c r="C34" s="56"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="55"/>
       <c r="E34" s="53"/>
     </row>
@@ -2002,8 +2009,8 @@
         <v>58</v>
       </c>
       <c r="B35" s="55"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="57"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="56"/>
       <c r="E35" s="53"/>
     </row>
     <row r="36">
@@ -2011,8 +2018,8 @@
         <v>59</v>
       </c>
       <c r="B36" s="55"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="57"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="56"/>
       <c r="E36" s="53"/>
     </row>
     <row r="37">
@@ -2020,8 +2027,8 @@
         <v>60</v>
       </c>
       <c r="B37" s="55"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="57"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="56"/>
       <c r="E37" s="53"/>
     </row>
     <row r="38">
@@ -2029,8 +2036,8 @@
         <v>61</v>
       </c>
       <c r="B38" s="55"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="57"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="53"/>
     </row>
     <row r="39">
@@ -2038,26 +2045,26 @@
         <v>62</v>
       </c>
       <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="57"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="56"/>
       <c r="E39" s="53"/>
     </row>
     <row r="40">
       <c r="A40" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="57"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="56"/>
       <c r="E40" s="53"/>
     </row>
     <row r="41">
-      <c r="A41" s="60" t="s">
+      <c r="A41" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="67"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="63"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="60"/>
       <c r="E41" s="53"/>
     </row>
     <row r="42">
@@ -2065,7 +2072,7 @@
         <v>65</v>
       </c>
       <c r="B42" s="51"/>
-      <c r="C42" s="64"/>
+      <c r="C42" s="66"/>
       <c r="D42" s="51"/>
       <c r="E42" s="53"/>
     </row>
@@ -2074,7 +2081,7 @@
         <v>66</v>
       </c>
       <c r="B43" s="55"/>
-      <c r="C43" s="56"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="55"/>
       <c r="E43" s="53"/>
     </row>
@@ -2092,7 +2099,7 @@
         <v>68</v>
       </c>
       <c r="B45" s="55"/>
-      <c r="C45" s="56"/>
+      <c r="C45" s="61"/>
       <c r="D45" s="55"/>
       <c r="E45" s="53"/>
     </row>
@@ -2101,7 +2108,7 @@
         <v>69</v>
       </c>
       <c r="B46" s="55"/>
-      <c r="C46" s="56"/>
+      <c r="C46" s="61"/>
       <c r="D46" s="55"/>
       <c r="E46" s="53"/>
     </row>
@@ -2110,8 +2117,8 @@
         <v>70</v>
       </c>
       <c r="B47" s="55"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="57"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="56"/>
       <c r="E47" s="53"/>
     </row>
     <row r="48">
@@ -2119,8 +2126,8 @@
         <v>71</v>
       </c>
       <c r="B48" s="55"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="57"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="56"/>
       <c r="E48" s="53"/>
     </row>
     <row r="49">
@@ -2128,8 +2135,8 @@
         <v>72</v>
       </c>
       <c r="B49" s="55"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="57"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="56"/>
       <c r="E49" s="53"/>
     </row>
     <row r="50">
@@ -2137,8 +2144,8 @@
         <v>73</v>
       </c>
       <c r="B50" s="55"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="57"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="56"/>
       <c r="E50" s="53"/>
     </row>
     <row r="51">
@@ -2146,26 +2153,26 @@
         <v>74</v>
       </c>
       <c r="B51" s="55"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="57"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="56"/>
       <c r="E51" s="53"/>
     </row>
     <row r="52">
       <c r="A52" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="B52" s="65"/>
-      <c r="C52" s="66"/>
-      <c r="D52" s="57"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="56"/>
       <c r="E52" s="53"/>
     </row>
     <row r="53">
-      <c r="A53" s="60" t="s">
+      <c r="A53" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="B53" s="67"/>
-      <c r="C53" s="68"/>
-      <c r="D53" s="63"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="60"/>
       <c r="E53" s="53"/>
     </row>
     <row r="54">
@@ -2173,7 +2180,7 @@
         <v>77</v>
       </c>
       <c r="B54" s="51"/>
-      <c r="C54" s="64"/>
+      <c r="C54" s="66"/>
       <c r="D54" s="51"/>
       <c r="E54" s="53"/>
     </row>
@@ -2182,7 +2189,7 @@
         <v>78</v>
       </c>
       <c r="B55" s="55"/>
-      <c r="C55" s="56"/>
+      <c r="C55" s="61"/>
       <c r="D55" s="55"/>
       <c r="E55" s="53"/>
     </row>
@@ -2191,7 +2198,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="55"/>
-      <c r="C56" s="56"/>
+      <c r="C56" s="61"/>
       <c r="D56" s="55"/>
       <c r="E56" s="53"/>
     </row>
@@ -2200,7 +2207,7 @@
         <v>80</v>
       </c>
       <c r="B57" s="55"/>
-      <c r="C57" s="56"/>
+      <c r="C57" s="61"/>
       <c r="D57" s="55"/>
       <c r="E57" s="53"/>
     </row>
@@ -2209,7 +2216,7 @@
         <v>81</v>
       </c>
       <c r="B58" s="55"/>
-      <c r="C58" s="56"/>
+      <c r="C58" s="61"/>
       <c r="D58" s="55"/>
       <c r="E58" s="53"/>
     </row>
@@ -2218,8 +2225,8 @@
         <v>82</v>
       </c>
       <c r="B59" s="55"/>
-      <c r="C59" s="56"/>
-      <c r="D59" s="57"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="56"/>
       <c r="E59" s="53"/>
     </row>
     <row r="60">
@@ -2227,8 +2234,8 @@
         <v>83</v>
       </c>
       <c r="B60" s="55"/>
-      <c r="C60" s="56"/>
-      <c r="D60" s="57"/>
+      <c r="C60" s="61"/>
+      <c r="D60" s="56"/>
       <c r="E60" s="53"/>
     </row>
     <row r="61">
@@ -2236,8 +2243,8 @@
         <v>84</v>
       </c>
       <c r="B61" s="55"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="57"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="56"/>
       <c r="E61" s="53"/>
     </row>
     <row r="62">
@@ -2245,8 +2252,8 @@
         <v>85</v>
       </c>
       <c r="B62" s="55"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="57"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="56"/>
       <c r="E62" s="53"/>
     </row>
     <row r="63">
@@ -2254,26 +2261,26 @@
         <v>86</v>
       </c>
       <c r="B63" s="55"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="57"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="56"/>
       <c r="E63" s="53"/>
     </row>
     <row r="64">
       <c r="A64" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="B64" s="65"/>
-      <c r="C64" s="66"/>
-      <c r="D64" s="57"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="56"/>
       <c r="E64" s="53"/>
     </row>
     <row r="65">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="B65" s="67"/>
-      <c r="C65" s="68"/>
-      <c r="D65" s="63"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="60"/>
       <c r="E65" s="53"/>
     </row>
     <row r="66">
@@ -2281,7 +2288,7 @@
         <v>89</v>
       </c>
       <c r="B66" s="51"/>
-      <c r="C66" s="64"/>
+      <c r="C66" s="66"/>
       <c r="D66" s="51"/>
       <c r="E66" s="53"/>
     </row>
@@ -2290,7 +2297,7 @@
         <v>90</v>
       </c>
       <c r="B67" s="55"/>
-      <c r="C67" s="56"/>
+      <c r="C67" s="61"/>
       <c r="D67" s="55"/>
       <c r="E67" s="53"/>
     </row>
@@ -2299,7 +2306,7 @@
         <v>91</v>
       </c>
       <c r="B68" s="55"/>
-      <c r="C68" s="56"/>
+      <c r="C68" s="61"/>
       <c r="D68" s="55"/>
       <c r="E68" s="53"/>
     </row>
@@ -2308,7 +2315,7 @@
         <v>92</v>
       </c>
       <c r="B69" s="55"/>
-      <c r="C69" s="56"/>
+      <c r="C69" s="61"/>
       <c r="D69" s="55"/>
       <c r="E69" s="53"/>
     </row>
@@ -2317,7 +2324,7 @@
         <v>93</v>
       </c>
       <c r="B70" s="55"/>
-      <c r="C70" s="56"/>
+      <c r="C70" s="61"/>
       <c r="D70" s="55"/>
       <c r="E70" s="53"/>
     </row>
@@ -2326,8 +2333,8 @@
         <v>94</v>
       </c>
       <c r="B71" s="55"/>
-      <c r="C71" s="56"/>
-      <c r="D71" s="57"/>
+      <c r="C71" s="61"/>
+      <c r="D71" s="56"/>
       <c r="E71" s="53"/>
     </row>
     <row r="72">
@@ -2335,8 +2342,8 @@
         <v>95</v>
       </c>
       <c r="B72" s="55"/>
-      <c r="C72" s="56"/>
-      <c r="D72" s="57"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="56"/>
       <c r="E72" s="53"/>
     </row>
     <row r="73">
@@ -2344,8 +2351,8 @@
         <v>96</v>
       </c>
       <c r="B73" s="55"/>
-      <c r="C73" s="56"/>
-      <c r="D73" s="57"/>
+      <c r="C73" s="61"/>
+      <c r="D73" s="56"/>
       <c r="E73" s="53"/>
     </row>
     <row r="74">
@@ -2353,8 +2360,8 @@
         <v>97</v>
       </c>
       <c r="B74" s="55"/>
-      <c r="C74" s="56"/>
-      <c r="D74" s="57"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="56"/>
       <c r="E74" s="53"/>
     </row>
     <row r="75">
@@ -2362,26 +2369,26 @@
         <v>98</v>
       </c>
       <c r="B75" s="55"/>
-      <c r="C75" s="56"/>
-      <c r="D75" s="57"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="56"/>
       <c r="E75" s="53"/>
     </row>
     <row r="76">
       <c r="A76" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="B76" s="65"/>
-      <c r="C76" s="66"/>
-      <c r="D76" s="57"/>
+      <c r="B76" s="62"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="56"/>
       <c r="E76" s="53"/>
     </row>
     <row r="77">
-      <c r="A77" s="60" t="s">
+      <c r="A77" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="B77" s="67"/>
-      <c r="C77" s="68"/>
-      <c r="D77" s="63"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="65"/>
+      <c r="D77" s="60"/>
       <c r="E77" s="53"/>
     </row>
   </sheetData>
@@ -2408,16 +2415,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="70" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="31" t="s">
@@ -2429,7 +2436,7 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="71" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="36">
@@ -2438,7 +2445,7 @@
       <c r="C2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D2" s="72">
         <v>43951.0</v>
       </c>
       <c r="E2" s="35" t="s">
@@ -2454,201 +2461,203 @@
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
-      <c r="F3" s="75"/>
+      <c r="F3" s="73"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="74" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="75" t="s">
         <v>103</v>
       </c>
       <c r="E4" s="41"/>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="76" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="79" t="s">
+      <c r="E5" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="80" t="s">
+      <c r="F5" s="78" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="82">
+      <c r="B6" s="80">
         <v>0.0466</v>
       </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83">
+      <c r="C6" s="80">
+        <v>0.043</v>
+      </c>
+      <c r="D6" s="81">
         <v>0.0253</v>
       </c>
-      <c r="E6" s="83">
+      <c r="E6" s="81">
         <v>0.0294</v>
       </c>
-      <c r="F6" s="84"/>
+      <c r="F6" s="82"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="83">
+      <c r="B7" s="81">
         <v>0.0304</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82">
-        <v>0.017</v>
-      </c>
-      <c r="E7" s="83">
+      <c r="C7" s="81">
+        <v>0.0241</v>
+      </c>
+      <c r="D7" s="80"/>
+      <c r="E7" s="81">
         <v>0.0184</v>
       </c>
-      <c r="F7" s="84"/>
+      <c r="F7" s="82"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="83">
+      <c r="B8" s="81">
         <v>0.0431</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82">
-        <v>0.0263</v>
-      </c>
-      <c r="E8" s="83">
+      <c r="C8" s="81">
+        <v>0.0387</v>
+      </c>
+      <c r="D8" s="80"/>
+      <c r="E8" s="81">
         <v>0.0298</v>
       </c>
-      <c r="F8" s="84"/>
+      <c r="F8" s="82"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="83">
+      <c r="B9" s="81">
         <v>0.0377</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82">
-        <v>0.0173</v>
-      </c>
-      <c r="E9" s="83">
+      <c r="C9" s="81">
+        <v>0.0282</v>
+      </c>
+      <c r="D9" s="80"/>
+      <c r="E9" s="81">
         <v>0.0253</v>
       </c>
-      <c r="F9" s="84"/>
+      <c r="F9" s="82"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="83">
+      <c r="B10" s="81">
         <v>0.0236</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82">
+      <c r="C10" s="81">
+        <v>0.0196</v>
+      </c>
+      <c r="D10" s="80"/>
+      <c r="E10" s="81">
         <v>0.0124</v>
       </c>
-      <c r="E10" s="83">
-        <v>0.0124</v>
-      </c>
-      <c r="F10" s="84"/>
+      <c r="F10" s="82"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="83" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="83">
+      <c r="B11" s="81">
         <v>0.0297</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82">
-        <v>0.0181</v>
-      </c>
-      <c r="E11" s="83">
+      <c r="C11" s="81">
+        <v>0.0268</v>
+      </c>
+      <c r="D11" s="80"/>
+      <c r="E11" s="81">
         <v>0.0213</v>
       </c>
-      <c r="F11" s="84"/>
+      <c r="F11" s="82"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="83">
+      <c r="B12" s="81">
         <v>0.0606</v>
       </c>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82">
-        <v>0.029</v>
-      </c>
-      <c r="E12" s="83">
+      <c r="C12" s="81">
+        <v>0.0574</v>
+      </c>
+      <c r="D12" s="80"/>
+      <c r="E12" s="81">
         <v>0.0332</v>
       </c>
-      <c r="F12" s="84"/>
+      <c r="F12" s="82"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="82">
+      <c r="B13" s="80">
         <v>0.0184</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82">
-        <v>0.0131</v>
-      </c>
-      <c r="E13" s="83">
+      <c r="C13" s="80">
+        <v>0.0163</v>
+      </c>
+      <c r="D13" s="80"/>
+      <c r="E13" s="81">
         <v>0.0165</v>
       </c>
-      <c r="F13" s="84"/>
+      <c r="F13" s="82"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="82">
+      <c r="B14" s="80">
         <v>0.042</v>
       </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82">
-        <v>0.0289</v>
-      </c>
-      <c r="E14" s="82">
+      <c r="C14" s="80">
+        <v>0.0404</v>
+      </c>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80">
         <v>0.0327</v>
       </c>
-      <c r="F14" s="84"/>
+      <c r="F14" s="82"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="83">
+      <c r="B15" s="81">
         <v>0.0613</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82">
-        <v>0.0319</v>
-      </c>
-      <c r="E15" s="83">
+      <c r="C15" s="81">
+        <v>0.0567</v>
+      </c>
+      <c r="D15" s="80"/>
+      <c r="E15" s="81">
         <v>0.0364</v>
       </c>
-      <c r="F15" s="84"/>
+      <c r="F15" s="82"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F6:F15">
@@ -2684,16 +2693,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="70" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="31" t="s">
@@ -2705,7 +2714,7 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="71" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="36">
@@ -2714,7 +2723,7 @@
       <c r="C2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D2" s="72">
         <v>43951.0</v>
       </c>
       <c r="E2" s="35" t="s">
@@ -2730,447 +2739,505 @@
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
-      <c r="F3" s="75"/>
+      <c r="F3" s="73"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="74" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="75" t="s">
         <v>103</v>
       </c>
       <c r="E4" s="41"/>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="76" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="79" t="s">
+      <c r="E5" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="80" t="s">
+      <c r="F5" s="78" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="85" t="s">
+      <c r="A6" s="84" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="86">
+      <c r="B6" s="85">
         <v>0.0314</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87">
+      <c r="C6" s="85">
+        <v>0.029</v>
+      </c>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86">
         <v>0.0232</v>
       </c>
-      <c r="F6" s="88"/>
+      <c r="F6" s="87"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="87">
+      <c r="B7" s="86">
         <v>0.0724</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87">
+      <c r="C7" s="86">
+        <v>0.0678</v>
+      </c>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86">
         <v>0.0387</v>
       </c>
-      <c r="F7" s="88"/>
+      <c r="F7" s="87"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="88" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="87">
+      <c r="B8" s="86">
         <v>0.0366</v>
       </c>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="87">
+      <c r="C8" s="86">
+        <v>0.0305</v>
+      </c>
+      <c r="D8" s="85"/>
+      <c r="E8" s="86">
         <v>0.027</v>
       </c>
-      <c r="F8" s="88"/>
+      <c r="F8" s="87"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="87">
+      <c r="B9" s="86">
         <v>0.0201</v>
       </c>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="87">
+      <c r="C9" s="86">
+        <v>0.0177</v>
+      </c>
+      <c r="D9" s="85"/>
+      <c r="E9" s="86">
         <v>0.0167</v>
       </c>
-      <c r="F9" s="88"/>
+      <c r="F9" s="87"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="88" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="87">
+      <c r="B10" s="86">
         <v>0.0632</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="87">
+      <c r="C10" s="86">
+        <v>0.0578</v>
+      </c>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86">
         <v>0.0409</v>
       </c>
-      <c r="F10" s="88"/>
+      <c r="F10" s="87"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="88" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="87">
+      <c r="B11" s="86">
         <v>0.0375</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="87">
+      <c r="C11" s="86">
+        <v>0.0355</v>
+      </c>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86">
         <v>0.0261</v>
       </c>
-      <c r="F11" s="88"/>
+      <c r="F11" s="87"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="88" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="87">
+      <c r="B12" s="86">
         <v>0.0281</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="87">
+      <c r="C12" s="86">
+        <v>0.0224</v>
+      </c>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86">
         <v>0.012</v>
       </c>
-      <c r="F12" s="88"/>
+      <c r="F12" s="87"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="B13" s="86">
+      <c r="B13" s="85">
         <v>0.0153</v>
       </c>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="87">
+      <c r="C13" s="85">
+        <v>0.0136</v>
+      </c>
+      <c r="D13" s="85"/>
+      <c r="E13" s="86">
         <v>0.0142</v>
       </c>
-      <c r="F13" s="88"/>
+      <c r="F13" s="87"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="88" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="86">
+      <c r="B14" s="85">
         <v>0.0135</v>
       </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86">
+      <c r="C14" s="85">
+        <v>0.0121</v>
+      </c>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85">
         <v>0.01</v>
       </c>
-      <c r="F14" s="88"/>
+      <c r="F14" s="87"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="88" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="87">
+      <c r="B15" s="86">
         <v>0.0607</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="87">
+      <c r="C15" s="86">
+        <v>0.0586</v>
+      </c>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86">
         <v>0.034</v>
       </c>
-      <c r="F15" s="88"/>
+      <c r="F15" s="87"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="88" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="87">
+      <c r="B16" s="86">
         <v>0.0586</v>
       </c>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="87">
+      <c r="C16" s="86">
+        <v>0.0543</v>
+      </c>
+      <c r="D16" s="85"/>
+      <c r="E16" s="86">
         <v>0.0295</v>
       </c>
-      <c r="F16" s="88"/>
+      <c r="F16" s="87"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="88" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="87">
+      <c r="B17" s="86">
         <v>0.0358</v>
       </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="87">
+      <c r="C17" s="86">
+        <v>0.0311</v>
+      </c>
+      <c r="D17" s="85"/>
+      <c r="E17" s="86">
         <v>0.023</v>
       </c>
-      <c r="F17" s="88"/>
+      <c r="F17" s="87"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="89" t="s">
+      <c r="A18" s="88" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="87">
+      <c r="B18" s="86">
         <v>0.0265</v>
       </c>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="87">
+      <c r="C18" s="86">
+        <v>0.023</v>
+      </c>
+      <c r="D18" s="85"/>
+      <c r="E18" s="86">
         <v>0.0168</v>
       </c>
-      <c r="F18" s="88"/>
+      <c r="F18" s="87"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="88" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="87">
+      <c r="B19" s="86">
         <v>0.0239</v>
       </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="87">
+      <c r="C19" s="86">
+        <v>0.0213</v>
+      </c>
+      <c r="D19" s="85"/>
+      <c r="E19" s="86">
         <v>0.0124</v>
       </c>
-      <c r="F19" s="88"/>
+      <c r="F19" s="87"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="89" t="s">
+      <c r="A20" s="88" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="87">
+      <c r="B20" s="86">
         <v>0.0447</v>
       </c>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="87">
+      <c r="C20" s="86">
+        <v>0.0408</v>
+      </c>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86">
         <v>0.0322</v>
       </c>
-      <c r="F20" s="88"/>
+      <c r="F20" s="87"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="89" t="s">
+      <c r="A21" s="88" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="87">
+      <c r="B21" s="86">
         <v>0.0148</v>
       </c>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="87">
+      <c r="C21" s="86">
+        <v>0.012</v>
+      </c>
+      <c r="D21" s="85"/>
+      <c r="E21" s="86">
         <v>0.0135</v>
       </c>
-      <c r="F21" s="88"/>
+      <c r="F21" s="87"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="89" t="s">
+      <c r="A22" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="87">
+      <c r="B22" s="86">
         <v>0.0219</v>
       </c>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="87">
+      <c r="C22" s="86">
+        <v>0.0164</v>
+      </c>
+      <c r="D22" s="85"/>
+      <c r="E22" s="86">
         <v>0.0199</v>
       </c>
-      <c r="F22" s="88"/>
+      <c r="F22" s="87"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="89" t="s">
+      <c r="A23" s="88" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="87">
+      <c r="B23" s="86">
         <v>0.0218</v>
       </c>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="87">
+      <c r="C23" s="86">
+        <v>0.0153</v>
+      </c>
+      <c r="D23" s="85"/>
+      <c r="E23" s="86">
         <v>0.0195</v>
       </c>
-      <c r="F23" s="88"/>
+      <c r="F23" s="87"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="89" t="s">
+      <c r="A24" s="88" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="87">
+      <c r="B24" s="86">
         <v>0.0508</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="87">
+      <c r="C24" s="86">
+        <v>0.0464</v>
+      </c>
+      <c r="D24" s="85"/>
+      <c r="E24" s="86">
         <v>0.0318</v>
       </c>
-      <c r="F24" s="88"/>
+      <c r="F24" s="87"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="89" t="s">
+      <c r="A25" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="B25" s="87">
+      <c r="B25" s="86">
         <v>0.0228</v>
       </c>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="87">
+      <c r="C25" s="86">
+        <v>0.0206</v>
+      </c>
+      <c r="D25" s="85"/>
+      <c r="E25" s="86">
         <v>0.0207</v>
       </c>
-      <c r="F25" s="88"/>
+      <c r="F25" s="87"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="89" t="s">
+      <c r="A26" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="87">
+      <c r="B26" s="86">
         <v>0.0316</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="87">
+      <c r="C26" s="86">
+        <v>0.0251</v>
+      </c>
+      <c r="D26" s="85"/>
+      <c r="E26" s="86">
         <v>0.0182</v>
       </c>
-      <c r="F26" s="88"/>
+      <c r="F26" s="87"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="B27" s="87">
+      <c r="B27" s="86">
         <v>0.0232</v>
       </c>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="87">
+      <c r="C27" s="86">
+        <v>0.021</v>
+      </c>
+      <c r="D27" s="85"/>
+      <c r="E27" s="86">
         <v>0.0196</v>
       </c>
-      <c r="F27" s="88"/>
+      <c r="F27" s="87"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="89" t="s">
+      <c r="A28" s="88" t="s">
         <v>143</v>
       </c>
-      <c r="B28" s="87">
+      <c r="B28" s="86">
         <v>0.0385</v>
       </c>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="87">
+      <c r="C28" s="86">
+        <v>0.0268</v>
+      </c>
+      <c r="D28" s="85"/>
+      <c r="E28" s="86">
         <v>0.0239</v>
       </c>
-      <c r="F28" s="88"/>
+      <c r="F28" s="87"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="89" t="s">
+      <c r="A29" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="87">
+      <c r="B29" s="86">
         <v>0.0378</v>
       </c>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="87">
+      <c r="C29" s="86">
+        <v>0.0324</v>
+      </c>
+      <c r="D29" s="85"/>
+      <c r="E29" s="86">
         <v>0.0257</v>
       </c>
-      <c r="F29" s="88"/>
+      <c r="F29" s="87"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="87">
+      <c r="B30" s="86">
         <v>0.021</v>
       </c>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="87">
+      <c r="C30" s="86">
+        <v>0.0187</v>
+      </c>
+      <c r="D30" s="85"/>
+      <c r="E30" s="86">
         <v>0.0183</v>
       </c>
-      <c r="F30" s="88"/>
+      <c r="F30" s="87"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="89" t="s">
+      <c r="A31" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="B31" s="87">
+      <c r="B31" s="86">
         <v>0.0472</v>
       </c>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="87">
+      <c r="C31" s="86">
+        <v>0.0457</v>
+      </c>
+      <c r="D31" s="85"/>
+      <c r="E31" s="86">
         <v>0.0365</v>
       </c>
-      <c r="F31" s="88"/>
+      <c r="F31" s="87"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="89" t="s">
+      <c r="A32" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="B32" s="87">
+      <c r="B32" s="86">
         <v>0.0215</v>
       </c>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="87">
+      <c r="C32" s="86">
+        <v>0.0184</v>
+      </c>
+      <c r="D32" s="85"/>
+      <c r="E32" s="86">
         <v>0.0126</v>
       </c>
-      <c r="F32" s="88"/>
+      <c r="F32" s="87"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="88" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="87">
+      <c r="B33" s="86">
         <v>0.0765</v>
       </c>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="87">
+      <c r="C33" s="86">
+        <v>0.0731</v>
+      </c>
+      <c r="D33" s="85"/>
+      <c r="E33" s="86">
         <v>0.0462</v>
       </c>
-      <c r="F33" s="88"/>
+      <c r="F33" s="87"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="89" t="s">
+      <c r="A34" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="87">
+      <c r="B34" s="86">
         <v>0.0657</v>
       </c>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
-      <c r="E34" s="87">
+      <c r="C34" s="86">
+        <v>0.0608</v>
+      </c>
+      <c r="D34" s="85"/>
+      <c r="E34" s="86">
         <v>0.0406</v>
       </c>
-      <c r="F34" s="88"/>
+      <c r="F34" s="87"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F6:F34">
@@ -3204,162 +3271,162 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="90" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="89" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="95"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="96"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="98"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="99"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="95"/>
+      <c r="A4" s="98"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="94"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="101"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="95"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="94"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="99"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="95"/>
+      <c r="A6" s="98"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="94"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="101"/>
-      <c r="B7" s="93"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="95"/>
+      <c r="A7" s="100"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="94"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="101"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="95"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="94"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="101"/>
-      <c r="B9" s="93"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="95"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="94"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="101"/>
-      <c r="B10" s="93"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="95"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="94"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="101"/>
-      <c r="B11" s="93"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="95"/>
+      <c r="A11" s="100"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="94"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="99"/>
-      <c r="B12" s="93"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="95"/>
+      <c r="A12" s="98"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="94"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="99"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="95"/>
+      <c r="A13" s="98"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="94"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="99"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="95"/>
+      <c r="A14" s="98"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="94"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="99"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="95"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="92"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="94"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="104"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="95"/>
+      <c r="A16" s="103"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="94"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="99"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="103"/>
-      <c r="D17" s="95"/>
+      <c r="A17" s="98"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="94"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="99"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="103"/>
-      <c r="D18" s="95"/>
+      <c r="A18" s="98"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="94"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="99"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="103"/>
-      <c r="D19" s="95"/>
+      <c r="A19" s="98"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="94"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="99"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="95"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="94"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="99"/>
-      <c r="B21" s="93"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="95"/>
+      <c r="A21" s="98"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="94"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="99"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="95"/>
+      <c r="A22" s="98"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="94"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="99"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="95"/>
+      <c r="A23" s="98"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="94"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="101"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="102"/>
-      <c r="D24" s="95"/>
+      <c r="A24" s="100"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="94"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="101"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="98"/>
+      <c r="A25" s="100"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="97"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>